<commit_message>
Self review and Code optimization
</commit_message>
<xml_diff>
--- a/com/test/resources/testData/TestData.xlsx
+++ b/com/test/resources/testData/TestData.xlsx
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,7 +204,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,7 +520,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -559,7 +558,7 @@
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -568,28 +567,28 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>